<commit_message>
Funcionalidades todas check Código HTML validado Código css validado
</commit_message>
<xml_diff>
--- a/Requisitos projecto 1.xlsx
+++ b/Requisitos projecto 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernardo\Desktop\AcertarORumo\Programação Avançada em Java\Projeto_1\projeto_scrum\scrum_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B1A513-9B9F-4D55-8B2C-6AE182907124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E77673-F127-44F6-A89F-30F653840A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>Catergoria</t>
   </si>
@@ -283,20 +283,17 @@
     <t>Bernardo</t>
   </si>
   <si>
-    <t>DA</t>
-  </si>
-  <si>
-    <t>CE</t>
-  </si>
-  <si>
-    <t>BE</t>
+    <t>Feito por:</t>
+  </si>
+  <si>
+    <t>Tabela das retrospetivas e atualização da informação impressa nesta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -319,8 +316,23 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,30 +373,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D2E9"/>
         <bgColor rgb="FFD9D2E9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -532,18 +520,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,7 +750,7 @@
   <dimension ref="A1:G1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -788,6 +772,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="27" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -799,17 +786,8 @@
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1">
@@ -822,17 +800,8 @@
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="23.25" customHeight="1">
@@ -845,8 +814,8 @@
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>27</v>
+      <c r="D4" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24.75" customHeight="1">
@@ -859,9 +828,10 @@
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>27</v>
       </c>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:7" ht="29.25" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -873,7 +843,7 @@
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -887,7 +857,7 @@
       <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>26</v>
       </c>
     </row>
@@ -901,7 +871,7 @@
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -915,7 +885,7 @@
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -929,9 +899,10 @@
       <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>27</v>
       </c>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" ht="21.75" customHeight="1">
       <c r="A11" s="6" t="s">
@@ -943,7 +914,7 @@
       <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -957,8 +928,8 @@
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>27</v>
+      <c r="D12" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="27" customHeight="1">
@@ -971,7 +942,7 @@
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="15" t="s">
         <v>26</v>
       </c>
     </row>
@@ -985,7 +956,7 @@
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -999,8 +970,8 @@
       <c r="C15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>25</v>
+      <c r="D15" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21.75" customHeight="1">
@@ -1013,8 +984,8 @@
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>26</v>
+      <c r="D16" s="15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.5" customHeight="1">
@@ -1027,67 +998,24 @@
       <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45.75" customHeight="1"/>
+    <row r="18" spans="1:4" ht="45.75" customHeight="1">
+      <c r="B18" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="19" spans="1:4" ht="42" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>26</v>
-      </c>
+      <c r="D19" s="15"/>
     </row>
-    <row r="20" spans="1:4" ht="42" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="39.6" customHeight="1">
-      <c r="A21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="36" customHeight="1">
-      <c r="A22" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
+    <row r="20" spans="1:4" ht="42" customHeight="1"/>
+    <row r="21" spans="1:4" ht="39.6" customHeight="1"/>
+    <row r="22" spans="1:4" ht="36" customHeight="1"/>
     <row r="23" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="25" spans="1:4" ht="15.75" customHeight="1"/>
@@ -2072,6 +2000,6 @@
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd"/>
+  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>